<commit_message>
29-ABR - 17:43 - JCSantos
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alicia LV\Downloads\REF_plantilla\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCSantos\Documents\UiPath\Contraportada_RPA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30566933-CC83-4638-BFB7-35C9390415D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA706F6-4803-47ED-B57F-B116746F4D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="14550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -152,28 +152,34 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>Trabajadores</t>
-  </si>
-  <si>
-    <t>aliciafilosofiamn@gmail.com's workspace</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>CredencialGmail</t>
-  </si>
-  <si>
     <t>EnvioCorreo</t>
   </si>
   <si>
     <t>ListKill</t>
   </si>
   <si>
-    <t>MiProceso</t>
-  </si>
-  <si>
     <t>EXCEL</t>
+  </si>
+  <si>
+    <t>Recomendaciones</t>
+  </si>
+  <si>
+    <t>nexusdatacorporation@gmail.com's workspace</t>
+  </si>
+  <si>
+    <t>Peticiones_Libros</t>
+  </si>
+  <si>
+    <t>CredentialGmail</t>
+  </si>
+  <si>
+    <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>CredentialCHATGPT</t>
   </si>
 </sst>
 </file>
@@ -549,18 +555,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -599,28 +605,28 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -636,21 +642,28 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1638,6 +1651,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1649,16 +1663,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1695,7 +1709,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1706,7 +1720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1820,7 +1834,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2812,16 +2826,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>